<commit_message>
Edited contact info, and testing git commit from Eclipse
</commit_message>
<xml_diff>
--- a/Admin/Team member contact info.xlsx
+++ b/Admin/Team member contact info.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Member Name</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>darciemilliken@gmail.com</t>
+  </si>
+  <si>
+    <t>jhatnguyen@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,6 +446,12 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>4039751270</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -452,8 +461,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>